<commit_message>
[FIX] zerobug: Re-enable coverage statistics
</commit_message>
<xml_diff>
--- a/z0bug_odoo/testenv/account_account.xlsx
+++ b/z0bug_odoo/testenv/account_account.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Tax Paid</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.bank</t>
+    <t xml:space="preserve">z0bug.coa_bank</t>
   </si>
   <si>
     <t xml:space="preserve">Bank</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">account.data_account_type_liquidity</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.cash</t>
+    <t xml:space="preserve">z0bug.coa_cash</t>
   </si>
   <si>
     <t xml:space="preserve">Cash</t>
@@ -546,7 +546,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,8 +1215,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>